<commit_message>
refs #881 refs #875
Former-commit-id: 2c111d1e2b2495f07dc3b0d32e2f6f3fbd224ad3
</commit_message>
<xml_diff>
--- a/doc/Bericht/05_Technischer Bericht/06_Hardware Evaluation & Tests/Anzahl Poster.xlsx
+++ b/doc/Bericht/05_Technischer Bericht/06_Hardware Evaluation & Tests/Anzahl Poster.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="FS 2008" sheetId="12" r:id="rId1"/>
@@ -40,9 +40,6 @@
     <t>Landschaftsarchitektur</t>
   </si>
   <si>
-    <t>Maschinentechnik | Innvation</t>
-  </si>
-  <si>
     <t>Raumplanung</t>
   </si>
   <si>
@@ -56,6 +53,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Maschinentechnik | Innovation</t>
   </si>
 </sst>
 </file>
@@ -96,7 +96,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -108,10 +108,1650 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-CH"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'FS 2008'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Anzahl Arbeiten</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'FS 2008'!$A$4:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Bauingenieurwesen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Elektrotechnik</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Informatik</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Landschaftsarchitektur</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maschinentechnik | Innovation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Raumplanung</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'FS 2008'!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-CH"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Gesamtübersicht!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Anzahl Arbeiten</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Gesamtübersicht!$A$4:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Bauingenieurwesen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Elektrotechnik</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Informatik</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Landschaftsarchitektur</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maschinentechnik | Innovation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Raumplanung</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Gesamtübersicht!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>134</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-CH"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HS 2008-2009'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Anzahl Arbeiten</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'HS 2008-2009'!$A$4:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Bauingenieurwesen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Elektrotechnik</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Informatik</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Landschaftsarchitektur</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maschinentechnik | Innovation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Raumplanung</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'HS 2008-2009'!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-CH"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'FS 2009'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Anzahl Arbeiten</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'FS 2009'!$A$4:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Bauingenieurwesen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Elektrotechnik</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Informatik</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Landschaftsarchitektur</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maschinentechnik | Innovation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Raumplanung</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'FS 2009'!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-CH"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HS 2009-2010'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Anzahl Arbeiten</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'HS 2009-2010'!$A$4:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Bauingenieurwesen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Elektrotechnik</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Informatik</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Landschaftsarchitektur</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maschinentechnik | Innovation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Raumplanung</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'HS 2009-2010'!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-CH"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'FS 2010'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Anzahl Arbeiten</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'FS 2010'!$A$4:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Bauingenieurwesen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Elektrotechnik</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Informatik</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Landschaftsarchitektur</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maschinentechnik | Innovation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Raumplanung</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'FS 2010'!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-CH"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HS 2010-2011'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Anzahl Arbeiten</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'HS 2010-2011'!$A$4:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Bauingenieurwesen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Elektrotechnik</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Informatik</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Landschaftsarchitektur</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maschinentechnik | Innovation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Raumplanung</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'HS 2010-2011'!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-CH"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'FS 2011'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Anzahl Arbeiten</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'FS 2011'!$A$4:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Bauingenieurwesen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Elektrotechnik</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Informatik</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Landschaftsarchitektur</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maschinentechnik | Innovation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Raumplanung</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'FS 2011'!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-CH"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HS 2011-2012'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Anzahl Arbeiten</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'HS 2011-2012'!$A$4:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Bauingenieurwesen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Elektrotechnik</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Informatik</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Landschaftsarchitektur</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maschinentechnik | Innovation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Raumplanung</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'HS 2011-2012'!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-CH"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'FS 2012'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Anzahl Arbeiten</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'FS 2012'!$A$4:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Bauingenieurwesen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Elektrotechnik</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Informatik</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Landschaftsarchitektur</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maschinentechnik | Innovation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Raumplanung</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'FS 2012'!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Diagramm 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -149,7 +1789,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -221,7 +1861,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -398,10 +2038,10 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
@@ -415,13 +2055,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -474,7 +2114,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>45</v>
@@ -486,7 +2126,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>21</v>
@@ -498,7 +2138,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <f>SUM(B4:B9)</f>
@@ -512,6 +2152,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -519,11 +2160,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
@@ -537,13 +2178,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -600,7 +2241,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <f>SUM('FS 2008'!B8,'HS 2008-2009'!B8,'FS 2009'!B8,'HS 2009-2010'!B8,'FS 2010'!B8,'HS 2010-2011'!B8,'FS 2011'!B8,'HS 2011-2012'!B8,'FS 2012'!B8)</f>
@@ -613,7 +2254,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <f>SUM('FS 2008'!B9,'HS 2008-2009'!B9,'FS 2009'!B9,'HS 2009-2010'!B9,'FS 2010'!B9,'HS 2010-2011'!B9,'FS 2011'!B9,'HS 2011-2012'!B9,'FS 2012'!B9)</f>
@@ -626,7 +2267,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <f>SUM(B4:B9)</f>
@@ -640,6 +2281,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -648,10 +2290,10 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
@@ -665,13 +2307,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -724,7 +2366,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -736,7 +2378,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -748,7 +2390,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <f>SUM(B4:B9)</f>
@@ -762,6 +2404,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -770,10 +2413,10 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
@@ -787,13 +2430,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -846,7 +2489,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>53</v>
@@ -858,7 +2501,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>24</v>
@@ -870,7 +2513,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <f>SUM(B4:B9)</f>
@@ -884,6 +2527,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -892,10 +2536,10 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
@@ -909,13 +2553,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -968,7 +2612,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>8</v>
@@ -980,7 +2624,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -992,7 +2636,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <f>SUM(B4:B9)</f>
@@ -1006,6 +2650,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1014,10 +2659,10 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
@@ -1031,13 +2676,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1090,7 +2735,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>50</v>
@@ -1102,7 +2747,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>33</v>
@@ -1114,7 +2759,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <f>SUM(B4:B9)</f>
@@ -1128,6 +2773,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1136,10 +2782,10 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
@@ -1153,13 +2799,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1212,7 +2858,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -1224,7 +2870,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1236,7 +2882,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <f>SUM(B4:B9)</f>
@@ -1250,6 +2896,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1257,11 +2904,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
@@ -1275,13 +2922,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1334,7 +2981,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>31</v>
@@ -1346,7 +2993,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>31</v>
@@ -1358,7 +3005,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <f>SUM(B4:B9)</f>
@@ -1372,6 +3019,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1380,10 +3028,10 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
@@ -1397,13 +3045,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1456,7 +3104,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>14</v>
@@ -1468,7 +3116,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1480,7 +3128,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <f>SUM(B4:B9)</f>
@@ -1494,6 +3142,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1502,10 +3151,10 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
@@ -1519,13 +3168,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1578,7 +3227,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>48</v>
@@ -1590,7 +3239,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>23</v>
@@ -1602,7 +3251,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <f>SUM(B4:B9)</f>
@@ -1616,5 +3265,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>